<commit_message>
multiple routes displayed && dronepanel layout
</commit_message>
<xml_diff>
--- a/json/GPS.xlsx
+++ b/json/GPS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Studienarbeit\github\Studienarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Studienarbeit\github\Studienarbeit\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7118E2CC-6BE1-42BB-BAEF-0085A5B9DCF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7E81F0-4D8C-47EA-AE55-806F18223804}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -7858,11 +7859,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -8221,14 +8223,14 @@
   <dimension ref="A1:W1425"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="59.42578125" customWidth="1"/>
-    <col min="14" max="14" width="65" customWidth="1"/>
+    <col min="14" max="14" width="105.42578125" customWidth="1"/>
     <col min="15" max="15" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8254,11 +8256,11 @@
       <c r="L1" s="3" t="s">
         <v>1225</v>
       </c>
-      <c r="N1" t="str">
+      <c r="N1" s="4" t="str">
         <f>RIGHT(L1,LEN(L1)-FIND(" ",L1,2))</f>
         <v>2019-05-20T20:29:00.000Z 54.31119090401512 10.131475925445558</v>
       </c>
-      <c r="O1" t="str">
+      <c r="O1" s="4" t="str">
         <f>LEFT(N1,FIND(" ",N1)-1)</f>
         <v>2019-05-20T20:29:00.000Z</v>
       </c>

</xml_diff>